<commit_message>
update qld and tqqq return
</commit_message>
<xml_diff>
--- a/qqq_qld_return.xlsx
+++ b/qqq_qld_return.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21600" windowHeight="9480"/>
+    <workbookView windowWidth="19200" windowHeight="6080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>holding_years</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>qld_return</t>
+  </si>
+  <si>
+    <t>tqqq_return</t>
   </si>
 </sst>
 </file>
@@ -673,11 +676,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -688,7 +691,7 @@
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
     <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
     <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
@@ -1026,20 +1029,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="14.4285714285714" customWidth="1"/>
-    <col min="2" max="3" width="12.8571428571429" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="1"/>
+    <col min="1" max="1" width="13.6363636363636" customWidth="1"/>
+    <col min="2" max="4" width="12.8181818181818" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1049,104 +1051,134 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>0.170493821285641</v>
+        <v>0.172725464013983</v>
       </c>
       <c r="C2" s="1">
-        <v>0.320084141912213</v>
+        <v>0.32380718115198</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.438057065078531</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>0.301433364266679</v>
+        <v>0.312276012629918</v>
       </c>
       <c r="C3" s="1">
-        <v>0.573226984142303</v>
+        <v>0.593909113633052</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.797561756343892</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>0.517408704046133</v>
+        <v>0.51889597120594</v>
       </c>
       <c r="C4" s="1">
-        <v>1.06805072414965</v>
+        <v>1.06809994620302</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1.51658129584604</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>1.00889281315861</v>
+        <v>1.03148385529191</v>
       </c>
       <c r="C5" s="1">
-        <v>2.22070817708846</v>
+        <v>2.29321491486981</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3.28179609241294</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>10</v>
       </c>
       <c r="B6" s="1">
-        <v>2.58845244841738</v>
+        <v>2.69324169105462</v>
       </c>
       <c r="C6" s="1">
-        <v>4.33292545123108</v>
+        <v>4.62879679790476</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4.83020106621927</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>15</v>
       </c>
       <c r="B7" s="1">
-        <v>4.68096998468697</v>
+        <v>4.8228797429133</v>
       </c>
       <c r="C7" s="1">
-        <v>8.71259835005675</v>
+        <v>9.33449855580181</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2.91128496484833</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>20</v>
       </c>
       <c r="B8" s="1">
-        <v>7.59060812912585</v>
+        <v>7.79636739815915</v>
       </c>
       <c r="C8" s="1">
-        <v>11.5727739670702</v>
+        <v>12.2610603510839</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2.19263625022717</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>25</v>
       </c>
       <c r="B9" s="1">
-        <v>16.6854566041452</v>
+        <v>16.2575243960344</v>
       </c>
       <c r="C9" s="1">
-        <v>42.1343128339482</v>
+        <v>40.5537579139876</v>
+      </c>
+      <c r="D9" s="1">
+        <v>12.5325406536171</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>30</v>
       </c>
       <c r="B10" s="1">
-        <v>38.3882046866406</v>
+        <v>39.1502108778063</v>
       </c>
       <c r="C10" s="1">
-        <v>177.712904346038</v>
+        <v>179.093558135726</v>
+      </c>
+      <c r="D10" s="1">
+        <v>84.8793314679889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>